<commit_message>
update readExcel class, Menu MN_9,10, forGotPassword Fp_1
</commit_message>
<xml_diff>
--- a/data/DataTestOnplus.xlsx
+++ b/data/DataTestOnplus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\automation-appium\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7157EBC2-5DB8-4534-944E-12578130C2AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4566A17B-93E0-4CC2-8499-1BBD1B2E06D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="1710" windowWidth="21600" windowHeight="12630" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
+    <workbookView xWindow="2790" yWindow="2400" windowWidth="21600" windowHeight="12630" activeTab="1" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="79">
   <si>
     <t>Test case</t>
   </si>
@@ -59,15 +59,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Tên</t>
-  </si>
-  <si>
-    <t>Ngày sinh</t>
-  </si>
-  <si>
-    <t>Giới tính</t>
-  </si>
-  <si>
     <t>PF_1</t>
   </si>
   <si>
@@ -155,12 +146,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>LG_1</t>
-  </si>
-  <si>
-    <t>LG_2</t>
-  </si>
-  <si>
     <t>LG_9</t>
   </si>
   <si>
@@ -221,15 +206,9 @@
     <t>LG_32</t>
   </si>
   <si>
-    <t>3/10/2024</t>
-  </si>
-  <si>
     <t>@gmail.com</t>
   </si>
   <si>
-    <t>PF_12</t>
-  </si>
-  <si>
     <t>PF_15</t>
   </si>
   <si>
@@ -237,6 +216,54 @@
   </si>
   <si>
     <t>123456</t>
+  </si>
+  <si>
+    <t>LG_1_2</t>
+  </si>
+  <si>
+    <t>LG_3</t>
+  </si>
+  <si>
+    <t>LG_4</t>
+  </si>
+  <si>
+    <t>LG_5</t>
+  </si>
+  <si>
+    <t>LG_37</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>autotest1@gmail.com</t>
+  </si>
+  <si>
+    <t>cuongVu</t>
+  </si>
+  <si>
+    <t>PF_6</t>
+  </si>
+  <si>
+    <t>vucuong@gmail.com</t>
+  </si>
+  <si>
+    <t>PF_7</t>
+  </si>
+  <si>
+    <t>autoTestOn@gmail.com</t>
+  </si>
+  <si>
+    <t>OTP</t>
+  </si>
+  <si>
+    <t>0399705143</t>
+  </si>
+  <si>
+    <t>121212</t>
   </si>
 </sst>
 </file>
@@ -350,9 +377,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -363,6 +387,9 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -680,247 +707,305 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4EEE9E-D85D-4BBC-BF3A-E5BE94229D24}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="31.140625" style="5" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="15"/>
+    </row>
+    <row r="3" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="15"/>
+    </row>
+    <row r="4" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="B8" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="B9" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="C9" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B10" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-    </row>
-    <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="B11" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="D14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
         <v>52</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>61</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="15"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="D18" s="8"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -930,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E6EDB0-492F-469B-9D93-054320C188DE}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,39 +1036,39 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4">
         <v>123456</v>
@@ -992,48 +1077,43 @@
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="10"/>
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1045,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F379703-D23D-4528-B95F-580E5D36195C}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,187 +1136,181 @@
     <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>12</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-    </row>
-    <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="4" t="s">
-        <v>20</v>
+      <c r="C5" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
-        <v>21</v>
+      <c r="C6" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="11" t="s">
-        <v>65</v>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
+        <v>20</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
+      <c r="D10" s="14" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F1CD6966-CF12-47B6-B282-DA0141A0D117}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{E9779CFA-97DA-40D0-87F0-27C88908B973}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{A46DB377-F0DD-4002-ADB9-7DCA4F4D7565}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{5A69DC2B-F697-452A-94AB-1BE090AAE136}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update thứ tự run case login, signUp_1,2,3
</commit_message>
<xml_diff>
--- a/data/DataTestOnplus.xlsx
+++ b/data/DataTestOnplus.xlsx
@@ -3,23 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\automation-appium\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4566A17B-93E0-4CC2-8499-1BBD1B2E06D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3149A7-1E93-4F85-A345-18E43EE6F2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="2400" windowWidth="21600" windowHeight="12630" activeTab="1" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
+    <workbookView xWindow="4050" yWindow="1680" windowWidth="21600" windowHeight="12450" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="ForgotPassword" sheetId="3" r:id="rId2"/>
-    <sheet name="Profile" sheetId="2" r:id="rId3"/>
+    <sheet name="SignUp" sheetId="4" r:id="rId2"/>
+    <sheet name="ForgotPassword" sheetId="3" r:id="rId3"/>
+    <sheet name="Profile" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="82">
   <si>
     <t>Test case</t>
   </si>
@@ -152,9 +153,6 @@
     <t>LG_10</t>
   </si>
   <si>
-    <t>0344888888</t>
-  </si>
-  <si>
     <t>LG_11</t>
   </si>
   <si>
@@ -167,109 +165,122 @@
     <t>LG_13</t>
   </si>
   <si>
+    <t>Tetson</t>
+  </si>
+  <si>
+    <t>Tets</t>
+  </si>
+  <si>
+    <t>AutoTest</t>
+  </si>
+  <si>
+    <t>@gmail.com</t>
+  </si>
+  <si>
+    <t>PF_15</t>
+  </si>
+  <si>
+    <t>nữ</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>LG_3</t>
+  </si>
+  <si>
+    <t>LG_4</t>
+  </si>
+  <si>
+    <t>LG_5</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>autotest1@gmail.com</t>
+  </si>
+  <si>
+    <t>cuongVu</t>
+  </si>
+  <si>
+    <t>PF_6</t>
+  </si>
+  <si>
+    <t>vucuong@gmail.com</t>
+  </si>
+  <si>
+    <t>PF_7</t>
+  </si>
+  <si>
+    <t>autoTestOn@gmail.com</t>
+  </si>
+  <si>
+    <t>OTP</t>
+  </si>
+  <si>
+    <t>0399705143</t>
+  </si>
+  <si>
+    <t>121212</t>
+  </si>
+  <si>
+    <t>LG_7_8</t>
+  </si>
+  <si>
+    <t>LG_1</t>
+  </si>
+  <si>
+    <t>LG_2</t>
+  </si>
+  <si>
+    <t>SU_1</t>
+  </si>
+  <si>
+    <t>SU_2</t>
+  </si>
+  <si>
+    <t>SU_3</t>
+  </si>
+  <si>
+    <t>SU_4</t>
+  </si>
+  <si>
+    <t>SU_5</t>
+  </si>
+  <si>
+    <t>SU_6</t>
+  </si>
+  <si>
+    <t>SU_7</t>
+  </si>
+  <si>
+    <t>SU_8</t>
+  </si>
+  <si>
+    <t>SU_9</t>
+  </si>
+  <si>
+    <t>0363964385</t>
+  </si>
+  <si>
     <t>LG_14</t>
   </si>
   <si>
-    <t>LG_21</t>
-  </si>
-  <si>
-    <t>LG_25</t>
-  </si>
-  <si>
-    <t>Tetson</t>
-  </si>
-  <si>
-    <t>LG_26</t>
-  </si>
-  <si>
-    <t>LG_27</t>
-  </si>
-  <si>
-    <t>LG_28</t>
-  </si>
-  <si>
-    <t>Tets</t>
-  </si>
-  <si>
-    <t>AutoTest</t>
-  </si>
-  <si>
-    <t>LG_29</t>
-  </si>
-  <si>
-    <t>LG_30</t>
-  </si>
-  <si>
-    <t>LG_31</t>
-  </si>
-  <si>
-    <t>LG_32</t>
-  </si>
-  <si>
-    <t>@gmail.com</t>
-  </si>
-  <si>
-    <t>PF_15</t>
-  </si>
-  <si>
-    <t>nữ</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>LG_1_2</t>
-  </si>
-  <si>
-    <t>LG_3</t>
-  </si>
-  <si>
-    <t>LG_4</t>
-  </si>
-  <si>
-    <t>LG_5</t>
-  </si>
-  <si>
-    <t>LG_37</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>autotest1@gmail.com</t>
-  </si>
-  <si>
-    <t>cuongVu</t>
-  </si>
-  <si>
-    <t>PF_6</t>
-  </si>
-  <si>
-    <t>vucuong@gmail.com</t>
-  </si>
-  <si>
-    <t>PF_7</t>
-  </si>
-  <si>
-    <t>autoTestOn@gmail.com</t>
-  </si>
-  <si>
-    <t>OTP</t>
-  </si>
-  <si>
-    <t>0399705143</t>
-  </si>
-  <si>
-    <t>121212</t>
+    <t/>
+  </si>
+  <si>
+    <t>0363991504</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -342,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -385,12 +396,15 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -707,22 +721,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4EEE9E-D85D-4BBC-BF3A-E5BE94229D24}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="6"/>
+    <col min="1" max="1" customWidth="true" style="2" width="21.42578125"/>
+    <col min="2" max="2" customWidth="true" style="2" width="15.85546875"/>
+    <col min="3" max="3" customWidth="true" style="5" width="31.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -732,280 +744,163 @@
       <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="15"/>
-    </row>
-    <row r="3" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="15"/>
-    </row>
-    <row r="4" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="15"/>
-    </row>
-    <row r="5" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="15"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B9" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="15"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="B10" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="20"/>
+    </row>
+    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="15"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="17" t="s">
+      <c r="B11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="15"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="15"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="15"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="15"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="20"/>
+    </row>
+    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="15"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="15"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="15"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="15"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="15"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="15"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="15"/>
+        <v>79</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="21">
+        <v>123456</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1014,18 +909,181 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E187E7C6-D9F5-4C98-A8B0-D3B346121D10}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="28.28515625"/>
+    <col min="2" max="2" customWidth="true" width="25.0"/>
+    <col min="3" max="3" customWidth="true" width="25.5703125"/>
+    <col min="4" max="4" customWidth="true" width="31.7109375"/>
+    <col min="5" max="5" customWidth="true" width="35.0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="3">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E6EDB0-492F-469B-9D93-054320C188DE}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="39.0"/>
+    <col min="2" max="2" customWidth="true" width="36.28515625"/>
+    <col min="3" max="3" customWidth="true" width="26.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
@@ -1123,7 +1181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F379703-D23D-4528-B95F-580E5D36195C}">
   <dimension ref="A1:J10"/>
   <sheetViews>
@@ -1133,10 +1191,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="20.7109375"/>
+    <col min="2" max="2" customWidth="true" width="20.0"/>
+    <col min="3" max="3" customWidth="true" width="22.42578125"/>
+    <col min="4" max="4" customWidth="true" width="29.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
@@ -1144,13 +1202,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -1184,10 +1242,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>13</v>
@@ -1217,11 +1275,11 @@
     </row>
     <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="11" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="7"/>
@@ -1233,11 +1291,11 @@
     </row>
     <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="11" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="7"/>
@@ -1285,7 +1343,7 @@
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="11" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="7"/>
@@ -1297,12 +1355,12 @@
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update Sign Up SU_4,5,6,7,8,9,10
</commit_message>
<xml_diff>
--- a/data/DataTestOnplus.xlsx
+++ b/data/DataTestOnplus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\automation-appium\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3149A7-1E93-4F85-A345-18E43EE6F2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AA4677-7A59-41A6-82E2-6456D13F98F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4050" yWindow="1680" windowWidth="21600" windowHeight="12450" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
+    <workbookView xWindow="2970" yWindow="3435" windowWidth="21735" windowHeight="12165" activeTab="1" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
   <si>
     <t>Test case</t>
   </si>
@@ -48,15 +48,6 @@
     <t>9363333666</t>
   </si>
   <si>
-    <t>AutoTest1#</t>
-  </si>
-  <si>
-    <t>Tetsonplus</t>
-  </si>
-  <si>
-    <t>Tetsonplus#</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -165,15 +156,6 @@
     <t>LG_13</t>
   </si>
   <si>
-    <t>Tetson</t>
-  </si>
-  <si>
-    <t>Tets</t>
-  </si>
-  <si>
-    <t>AutoTest</t>
-  </si>
-  <si>
     <t>@gmail.com</t>
   </si>
   <si>
@@ -237,12 +219,6 @@
     <t>LG_2</t>
   </si>
   <si>
-    <t>SU_1</t>
-  </si>
-  <si>
-    <t>SU_2</t>
-  </si>
-  <si>
     <t>SU_3</t>
   </si>
   <si>
@@ -252,28 +228,79 @@
     <t>SU_5</t>
   </si>
   <si>
+    <t>LG_14</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0363991504</t>
+  </si>
+  <si>
+    <t>SU_10</t>
+  </si>
+  <si>
+    <t>SU_11</t>
+  </si>
+  <si>
+    <t>SU_12</t>
+  </si>
+  <si>
+    <t>SU_13</t>
+  </si>
+  <si>
+    <t>SU_14</t>
+  </si>
+  <si>
+    <t>SU_15</t>
+  </si>
+  <si>
+    <t>SU_16</t>
+  </si>
+  <si>
+    <t>SU_17</t>
+  </si>
+  <si>
+    <t>autotest1</t>
+  </si>
+  <si>
+    <t>1234A</t>
+  </si>
+  <si>
+    <t>auto123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t>Autotest1#</t>
+  </si>
+  <si>
+    <t>autotest12</t>
+  </si>
+  <si>
     <t>SU_6</t>
   </si>
   <si>
-    <t>SU_7</t>
-  </si>
-  <si>
-    <t>SU_8</t>
-  </si>
-  <si>
     <t>SU_9</t>
   </si>
   <si>
-    <t>0363964385</t>
-  </si>
-  <si>
-    <t>LG_14</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>0363991504</t>
+    <t>SU_7_8</t>
+  </si>
+  <si>
+    <t>SU_1_2</t>
+  </si>
+  <si>
+    <t>0363273271</t>
+  </si>
+  <si>
+    <t>848346</t>
+  </si>
+  <si>
+    <t>903649</t>
+  </si>
+  <si>
+    <t>0363894985</t>
   </si>
 </sst>
 </file>
@@ -353,7 +380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -397,9 +424,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -723,7 +747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4EEE9E-D85D-4BBC-BF3A-E5BE94229D24}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -739,74 +763,74 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>67</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>80</v>
+        <v>35</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>80</v>
+        <v>35</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>80</v>
+        <v>35</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>3</v>
@@ -814,91 +838,91 @@
       <c r="C6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="20" t="s">
-        <v>80</v>
+      <c r="D6" s="19" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>80</v>
+        <v>45</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="20"/>
+        <v>45</v>
+      </c>
+      <c r="D8" s="19"/>
     </row>
     <row r="9" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="20"/>
+        <v>45</v>
+      </c>
+      <c r="D9" s="19"/>
     </row>
     <row r="10" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="20"/>
+        <v>45</v>
+      </c>
+      <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>80</v>
+        <v>59</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C12" s="17"/>
-      <c r="D12" s="20"/>
+      <c r="D12" s="19"/>
     </row>
     <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="21">
+      <c r="D13" s="20">
         <v>123456</v>
       </c>
     </row>
@@ -910,10 +934,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E187E7C6-D9F5-4C98-A8B0-D3B346121D10}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,148 +950,227 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="3">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>70</v>
-      </c>
       <c r="B3" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="3" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>72</v>
+      <c r="A5" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>73</v>
+      <c r="A6" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="C6" s="4"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="A7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>75</v>
+      <c r="A8" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="8"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="4">
+        <v>123456</v>
+      </c>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1076,7 +1179,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,39 +1197,39 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" s="4">
         <v>123456</v>
@@ -1135,42 +1238,42 @@
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1202,13 +1305,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -1219,16 +1322,16 @@
     </row>
     <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -1239,16 +1342,16 @@
     </row>
     <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -1259,10 +1362,10 @@
     </row>
     <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1275,11 +1378,11 @@
     </row>
     <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="7"/>
@@ -1291,11 +1394,11 @@
     </row>
     <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="7"/>
@@ -1307,11 +1410,11 @@
     </row>
     <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="7"/>
@@ -1323,11 +1426,11 @@
     </row>
     <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="7"/>
@@ -1339,11 +1442,11 @@
     </row>
     <row r="9" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="7"/>
@@ -1355,12 +1458,12 @@
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update Sign Up SU_11,12,13,14,15,16,17,18,19
</commit_message>
<xml_diff>
--- a/data/DataTestOnplus.xlsx
+++ b/data/DataTestOnplus.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\automation-appium\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AA4677-7A59-41A6-82E2-6456D13F98F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D92773-804E-42C5-BE4A-23B7570CB44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="3435" windowWidth="21735" windowHeight="12165" activeTab="1" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
+    <workbookView xWindow="4275" yWindow="2295" windowWidth="21735" windowHeight="12165" activeTab="2" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="93">
   <si>
     <t>Test case</t>
   </si>
@@ -93,9 +93,6 @@
     <t>FP_8</t>
   </si>
   <si>
-    <t>auto12</t>
-  </si>
-  <si>
     <t>FP_9</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
     <t>OTP</t>
   </si>
   <si>
-    <t>0399705143</t>
-  </si>
-  <si>
     <t>121212</t>
   </si>
   <si>
@@ -234,9 +228,6 @@
     <t/>
   </si>
   <si>
-    <t>0363991504</t>
-  </si>
-  <si>
     <t>SU_10</t>
   </si>
   <si>
@@ -291,24 +282,38 @@
     <t>SU_1_2</t>
   </si>
   <si>
-    <t>0363273271</t>
-  </si>
-  <si>
-    <t>848346</t>
-  </si>
-  <si>
-    <t>903649</t>
-  </si>
-  <si>
-    <t>0363894985</t>
+    <t>0363788226</t>
+  </si>
+  <si>
+    <t>0363863211</t>
+  </si>
+  <si>
+    <t>SU_18</t>
+  </si>
+  <si>
+    <t>0363105890</t>
+  </si>
+  <si>
+    <t>374958</t>
+  </si>
+  <si>
+    <t>614772</t>
+  </si>
+  <si>
+    <t>888952</t>
+  </si>
+  <si>
+    <t>FP_1</t>
+  </si>
+  <si>
+    <t>FP_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,8 +342,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,6 +359,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,7 +397,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -428,6 +445,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -753,9 +792,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="21.42578125"/>
-    <col min="2" max="2" customWidth="true" style="2" width="15.85546875"/>
-    <col min="3" max="3" customWidth="true" style="5" width="31.140625"/>
+    <col min="1" max="1" width="21.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
@@ -763,74 +802,74 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>3</v>
@@ -839,86 +878,86 @@
         <v>2</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="19"/>
     </row>
     <row r="9" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="19"/>
     </row>
     <row r="10" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="19"/>
     </row>
     <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -936,17 +975,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E187E7C6-D9F5-4C98-A8B0-D3B346121D10}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.28515625"/>
-    <col min="2" max="2" customWidth="true" width="25.0"/>
-    <col min="3" max="3" customWidth="true" width="25.5703125"/>
-    <col min="4" max="4" customWidth="true" width="31.7109375"/>
-    <col min="5" max="5" customWidth="true" width="35.0"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -954,55 +993,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>87</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1013,7 +1052,7 @@
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1024,7 +1063,7 @@
     </row>
     <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1035,7 +1074,7 @@
     </row>
     <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1046,127 +1085,133 @@
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>45</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D12" s="4"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="4">
-        <v>123456</v>
+        <v>57</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+    <row r="17" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1176,109 +1221,192 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E6EDB0-492F-469B-9D93-054320C188DE}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.0"/>
-    <col min="2" max="2" customWidth="true" width="36.28515625"/>
-    <col min="3" max="3" customWidth="true" width="26.28515625"/>
+    <col min="1" max="2" width="39" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+    </row>
+    <row r="2" spans="1:15" s="24" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+    </row>
+    <row r="3" spans="1:15" s="24" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23">
+        <v>657758</v>
+      </c>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+    </row>
+    <row r="4" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+    </row>
+    <row r="5" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="30"/>
+    </row>
+    <row r="6" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="30"/>
+    </row>
+    <row r="7" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4">
+        <v>123456</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="30"/>
+    </row>
+    <row r="8" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="30"/>
+    </row>
+    <row r="9" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="30"/>
+    </row>
+    <row r="10" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="10"/>
-    </row>
-    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="10"/>
-    </row>
-    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="4">
-        <v>123456</v>
-      </c>
-      <c r="C5" s="10"/>
-    </row>
-    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="10"/>
-    </row>
-    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="D10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="30"/>
+    </row>
+    <row r="11" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="D11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="30"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="auto@" xr:uid="{F9A5EFC1-176C-4015-A1D3-4097A6E9F144}"/>
+    <hyperlink ref="C6" r:id="rId1" display="auto@" xr:uid="{F9A5EFC1-176C-4015-A1D3-4097A6E9F144}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1294,10 +1422,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="20.7109375"/>
-    <col min="2" max="2" customWidth="true" width="20.0"/>
-    <col min="3" max="3" customWidth="true" width="22.42578125"/>
-    <col min="4" max="4" customWidth="true" width="29.7109375"/>
+    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
@@ -1305,13 +1433,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -1345,10 +1473,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
@@ -1378,11 +1506,11 @@
     </row>
     <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="7"/>
@@ -1394,11 +1522,11 @@
     </row>
     <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="7"/>
@@ -1446,7 +1574,7 @@
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="7"/>
@@ -1458,12 +1586,12 @@
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update forgot pass word FP_10,11,12,13,14,15,16,17,18
</commit_message>
<xml_diff>
--- a/data/DataTestOnplus.xlsx
+++ b/data/DataTestOnplus.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\automation-appium\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D92773-804E-42C5-BE4A-23B7570CB44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC14D85D-A454-4788-B917-2D5E9B04368A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="2295" windowWidth="21735" windowHeight="12165" activeTab="2" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
+    <workbookView xWindow="540" yWindow="2355" windowWidth="21000" windowHeight="12165" activeTab="2" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="102">
   <si>
     <t>Test case</t>
   </si>
@@ -96,18 +96,12 @@
     <t>FP_9</t>
   </si>
   <si>
-    <t>autot</t>
-  </si>
-  <si>
     <t>FP_10</t>
   </si>
   <si>
     <t>FP_11</t>
   </si>
   <si>
-    <t xml:space="preserve">       </t>
-  </si>
-  <si>
     <t>FP_12</t>
   </si>
   <si>
@@ -291,28 +285,62 @@
     <t>SU_18</t>
   </si>
   <si>
-    <t>0363105890</t>
-  </si>
-  <si>
-    <t>374958</t>
-  </si>
-  <si>
-    <t>614772</t>
-  </si>
-  <si>
-    <t>888952</t>
-  </si>
-  <si>
     <t>FP_1</t>
   </si>
   <si>
     <t>FP_2</t>
+  </si>
+  <si>
+    <t>0363242215</t>
+  </si>
+  <si>
+    <t>897576</t>
+  </si>
+  <si>
+    <t>860624</t>
+  </si>
+  <si>
+    <t>914223</t>
+  </si>
+  <si>
+    <t>12345a</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>FP_3</t>
+  </si>
+  <si>
+    <t>FP_15_16</t>
+  </si>
+  <si>
+    <t>FP_17</t>
+  </si>
+  <si>
+    <t>0363789999</t>
+  </si>
+  <si>
+    <t>657758</t>
+  </si>
+  <si>
+    <t>AutoTest!8</t>
+  </si>
+  <si>
+    <t>AutoTest?1</t>
+  </si>
+  <si>
+    <t>AutoTest#5</t>
+  </si>
+  <si>
+    <t>AutoTest(1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -336,15 +364,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="13"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -397,7 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -420,7 +446,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -458,16 +483,11 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -792,176 +812,176 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="5" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="21.42578125"/>
+    <col min="2" max="2" customWidth="true" style="2" width="15.85546875"/>
+    <col min="3" max="3" customWidth="true" style="5" width="31.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="17" t="s">
+      <c r="B8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="18"/>
+    </row>
+    <row r="9" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="18" t="s">
+      <c r="B9" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="17" t="s">
+      <c r="C9" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="18"/>
+    </row>
+    <row r="10" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="19"/>
-    </row>
-    <row r="9" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="C10" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="18"/>
+    </row>
+    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="19"/>
-    </row>
-    <row r="10" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="B11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="19"/>
+      <c r="B12" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="18"/>
     </row>
     <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>64</v>
+      <c r="A13" s="14" t="s">
+        <v>62</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="20">
+      <c r="D13" s="19">
         <v>123456</v>
       </c>
     </row>
@@ -981,67 +1001,67 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="35" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="28.28515625"/>
+    <col min="2" max="2" customWidth="true" width="25.0"/>
+    <col min="3" max="3" customWidth="true" width="25.5703125"/>
+    <col min="4" max="4" customWidth="true" width="31.7109375"/>
+    <col min="5" max="5" customWidth="true" width="35.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>56</v>
+      <c r="D1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>87</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1052,7 +1072,7 @@
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1063,7 +1083,7 @@
     </row>
     <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1074,7 +1094,7 @@
     </row>
     <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1085,7 +1105,7 @@
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1096,122 +1116,122 @@
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B17" s="21"/>
+        <v>84</v>
+      </c>
+      <c r="B17" s="20"/>
       <c r="C17" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="21"/>
+        <v>42</v>
+      </c>
+      <c r="E17" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1221,194 +1241,256 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E6EDB0-492F-469B-9D93-054320C188DE}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="5"/>
+    <col min="1" max="1" customWidth="true" width="39.0"/>
+    <col min="2" max="2" customWidth="true" width="29.5703125"/>
+    <col min="3" max="3" customWidth="true" width="36.28515625"/>
+    <col min="4" max="4" customWidth="true" width="26.28515625"/>
+    <col min="5" max="5" style="5" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-    </row>
-    <row r="2" spans="1:15" s="24" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="D1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="23" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="23" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="23" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-    </row>
-    <row r="3" spans="1:15" s="24" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="D7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23">
-        <v>657758</v>
-      </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-    </row>
-    <row r="4" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-    </row>
-    <row r="5" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="30"/>
-    </row>
-    <row r="6" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="30"/>
-    </row>
-    <row r="7" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="D8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4">
-        <v>123456</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="30"/>
-    </row>
-    <row r="8" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="B9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4" t="s">
+      <c r="B10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="30"/>
-    </row>
-    <row r="9" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="D10" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4" t="s">
+      <c r="B11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="30"/>
-    </row>
-    <row r="10" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="30"/>
-    </row>
-    <row r="11" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="30"/>
+      <c r="E12" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" display="auto@" xr:uid="{F9A5EFC1-176C-4015-A1D3-4097A6E9F144}"/>
+    <hyperlink ref="C7" r:id="rId1" display="auto@" xr:uid="{F9A5EFC1-176C-4015-A1D3-4097A6E9F144}"/>
+    <hyperlink ref="C8" r:id="rId2" display="auto@" xr:uid="{9F6E0FC7-C05D-474B-854D-64E9E0501095}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1422,24 +1504,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="20.7109375"/>
+    <col min="2" max="2" customWidth="true" width="20.0"/>
+    <col min="3" max="3" customWidth="true" width="22.42578125"/>
+    <col min="4" max="4" customWidth="true" width="29.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>49</v>
+      <c r="D1" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -1455,7 +1537,7 @@
       <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1473,10 +1555,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
@@ -1506,11 +1588,11 @@
     </row>
     <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="11" t="s">
-        <v>53</v>
+      <c r="C5" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="7"/>
@@ -1522,11 +1604,11 @@
     </row>
     <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="11" t="s">
-        <v>55</v>
+      <c r="C6" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="7"/>
@@ -1573,8 +1655,8 @@
         <v>17</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="11" t="s">
-        <v>41</v>
+      <c r="C9" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="7"/>
@@ -1586,12 +1668,12 @@
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update signUp 20, test app on browser stack
</commit_message>
<xml_diff>
--- a/data/DataTestOnplus.xlsx
+++ b/data/DataTestOnplus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\automation-appium\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC14D85D-A454-4788-B917-2D5E9B04368A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6E2D14-DF73-405D-8945-CE3DDB0423CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="2355" windowWidth="21000" windowHeight="12165" activeTab="2" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
+    <workbookView xWindow="690" yWindow="1545" windowWidth="21000" windowHeight="12165" activeTab="1" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="108">
   <si>
     <t>Test case</t>
   </si>
@@ -279,9 +279,6 @@
     <t>0363788226</t>
   </si>
   <si>
-    <t>0363863211</t>
-  </si>
-  <si>
     <t>SU_18</t>
   </si>
   <si>
@@ -291,15 +288,6 @@
     <t>FP_2</t>
   </si>
   <si>
-    <t>0363242215</t>
-  </si>
-  <si>
-    <t>897576</t>
-  </si>
-  <si>
-    <t>860624</t>
-  </si>
-  <si>
     <t>914223</t>
   </si>
   <si>
@@ -324,16 +312,46 @@
     <t>657758</t>
   </si>
   <si>
-    <t>AutoTest!8</t>
-  </si>
-  <si>
-    <t>AutoTest?1</t>
-  </si>
-  <si>
     <t>AutoTest#5</t>
   </si>
   <si>
     <t>AutoTest(1</t>
+  </si>
+  <si>
+    <t>0363697350</t>
+  </si>
+  <si>
+    <t>0363423791</t>
+  </si>
+  <si>
+    <t>261050</t>
+  </si>
+  <si>
+    <t>543907</t>
+  </si>
+  <si>
+    <t>0363932944</t>
+  </si>
+  <si>
+    <t>0363299733</t>
+  </si>
+  <si>
+    <t>518062</t>
+  </si>
+  <si>
+    <t>748241</t>
+  </si>
+  <si>
+    <t>0363285179</t>
+  </si>
+  <si>
+    <t>417116</t>
+  </si>
+  <si>
+    <t>805154</t>
+  </si>
+  <si>
+    <t>668334</t>
   </si>
 </sst>
 </file>
@@ -970,7 +988,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="18"/>
@@ -995,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E187E7C6-D9F5-4C98-A8B0-D3B346121D10}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,7 +1048,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>63</v>
@@ -1067,7 +1085,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="8"/>
       <c r="E4" s="3" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1078,7 +1096,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="8"/>
       <c r="E5" s="3" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1089,7 +1107,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="8"/>
       <c r="E6" s="3" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1100,7 +1118,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="8"/>
       <c r="E7" s="3" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1111,7 +1129,7 @@
       <c r="C8" s="4"/>
       <c r="D8" s="8"/>
       <c r="E8" s="3" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1222,7 +1240,7 @@
     </row>
     <row r="17" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="4" t="s">
@@ -1243,7 +1261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E6EDB0-492F-469B-9D93-054320C188DE}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1275,10 +1293,10 @@
     </row>
     <row r="2" spans="1:5" s="23" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>63</v>
@@ -1292,7 +1310,7 @@
     </row>
     <row r="3" spans="1:5" s="23" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>63</v>
@@ -1304,15 +1322,15 @@
         <v>63</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="23" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>63</v>
@@ -1358,7 +1376,7 @@
         <v>63</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>63</v>
@@ -1375,7 +1393,7 @@
         <v>63</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>63</v>
@@ -1454,16 +1472,16 @@
     </row>
     <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>63</v>
@@ -1471,16 +1489,16 @@
     </row>
     <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E14" s="9"/>
     </row>

</xml_diff>

<commit_message>
update base, test signUp browserStack
</commit_message>
<xml_diff>
--- a/data/DataTestOnplus.xlsx
+++ b/data/DataTestOnplus.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="116">
   <si>
     <t>Test case</t>
   </si>
@@ -352,6 +352,30 @@
   </si>
   <si>
     <t>668334</t>
+  </si>
+  <si>
+    <t>0363683445</t>
+  </si>
+  <si>
+    <t>922734</t>
+  </si>
+  <si>
+    <t>752110</t>
+  </si>
+  <si>
+    <t>958279</t>
+  </si>
+  <si>
+    <t>0363976205</t>
+  </si>
+  <si>
+    <t>0363870101</t>
+  </si>
+  <si>
+    <t>0363837692</t>
+  </si>
+  <si>
+    <t>0363714939</t>
   </si>
 </sst>
 </file>
@@ -988,7 +1012,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="18"/>
@@ -1048,7 +1072,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>63</v>
@@ -1085,7 +1109,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="8"/>
       <c r="E4" s="3" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1096,7 +1120,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="8"/>
       <c r="E5" s="3" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1107,7 +1131,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="8"/>
       <c r="E6" s="3" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1118,7 +1142,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="8"/>
       <c r="E7" s="3" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1129,7 +1153,7 @@
       <c r="C8" s="4"/>
       <c r="D8" s="8"/>
       <c r="E8" s="3" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update search test SA_1->10
</commit_message>
<xml_diff>
--- a/data/DataTestOnplus.xlsx
+++ b/data/DataTestOnplus.xlsx
@@ -3,24 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\automation-appium\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6E2D14-DF73-405D-8945-CE3DDB0423CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E057D3-AAD7-4FBC-B6B9-FD861CCED63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="1545" windowWidth="21000" windowHeight="12165" activeTab="1" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
+    <workbookView xWindow="9030" yWindow="2505" windowWidth="21000" windowHeight="12165" activeTab="4" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="SignUp" sheetId="4" r:id="rId2"/>
     <sheet name="ForgotPassword" sheetId="3" r:id="rId3"/>
     <sheet name="Profile" sheetId="2" r:id="rId4"/>
+    <sheet name="Search" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="128">
   <si>
     <t>Test case</t>
   </si>
@@ -288,9 +289,6 @@
     <t>FP_2</t>
   </si>
   <si>
-    <t>914223</t>
-  </si>
-  <si>
     <t>12345a</t>
   </si>
   <si>
@@ -318,45 +316,6 @@
     <t>AutoTest(1</t>
   </si>
   <si>
-    <t>0363697350</t>
-  </si>
-  <si>
-    <t>0363423791</t>
-  </si>
-  <si>
-    <t>261050</t>
-  </si>
-  <si>
-    <t>543907</t>
-  </si>
-  <si>
-    <t>0363932944</t>
-  </si>
-  <si>
-    <t>0363299733</t>
-  </si>
-  <si>
-    <t>518062</t>
-  </si>
-  <si>
-    <t>748241</t>
-  </si>
-  <si>
-    <t>0363285179</t>
-  </si>
-  <si>
-    <t>417116</t>
-  </si>
-  <si>
-    <t>805154</t>
-  </si>
-  <si>
-    <t>668334</t>
-  </si>
-  <si>
-    <t>0363683445</t>
-  </si>
-  <si>
     <t>922734</t>
   </si>
   <si>
@@ -366,23 +325,100 @@
     <t>958279</t>
   </si>
   <si>
-    <t>0363976205</t>
-  </si>
-  <si>
     <t>0363870101</t>
   </si>
   <si>
-    <t>0363837692</t>
-  </si>
-  <si>
     <t>0363714939</t>
+  </si>
+  <si>
+    <t>SA_1_2</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>SA_3</t>
+  </si>
+  <si>
+    <t>SA_4</t>
+  </si>
+  <si>
+    <t>SA_5</t>
+  </si>
+  <si>
+    <t>SA_6</t>
+  </si>
+  <si>
+    <t>SA_7</t>
+  </si>
+  <si>
+    <t>SA_8</t>
+  </si>
+  <si>
+    <t>SA_9</t>
+  </si>
+  <si>
+    <t>SA_10</t>
+  </si>
+  <si>
+    <t>SA_11</t>
+  </si>
+  <si>
+    <t>SA_12</t>
+  </si>
+  <si>
+    <t>Kênh ANTV</t>
+  </si>
+  <si>
+    <t>Sự kiện giải đấu Wcup</t>
+  </si>
+  <si>
+    <t>THỂ THAO VIỆT</t>
+  </si>
+  <si>
+    <t>THE THAO VIET</t>
+  </si>
+  <si>
+    <t>the thao viet</t>
+  </si>
+  <si>
+    <t>Hightlights La Liga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kênh </t>
+  </si>
+  <si>
+    <t>Nhà vô địch</t>
+  </si>
+  <si>
+    <t>SA_13</t>
+  </si>
+  <si>
+    <t>SA_14</t>
+  </si>
+  <si>
+    <t>Kênh VTV</t>
+  </si>
+  <si>
+    <t>SA_15</t>
+  </si>
+  <si>
+    <t>Sự kiện</t>
+  </si>
+  <si>
+    <t>Highlights</t>
+  </si>
+  <si>
+    <t>Highlights - Serie A</t>
+  </si>
+  <si>
+    <t>[k+] su kien k+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -465,7 +501,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -530,6 +566,9 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -854,9 +893,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="21.42578125"/>
-    <col min="2" max="2" customWidth="true" style="2" width="15.85546875"/>
-    <col min="3" max="3" customWidth="true" style="5" width="31.140625"/>
+    <col min="1" max="1" width="21.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
@@ -1012,7 +1051,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="18"/>
@@ -1037,17 +1076,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E187E7C6-D9F5-4C98-A8B0-D3B346121D10}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.28515625"/>
-    <col min="2" max="2" customWidth="true" width="25.0"/>
-    <col min="3" max="3" customWidth="true" width="25.5703125"/>
-    <col min="4" max="4" customWidth="true" width="31.7109375"/>
-    <col min="5" max="5" customWidth="true" width="35.0"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1072,7 +1111,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>63</v>
@@ -1109,7 +1148,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="8"/>
       <c r="E4" s="3" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1120,7 +1159,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="8"/>
       <c r="E5" s="3" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1131,7 +1170,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="8"/>
       <c r="E6" s="3" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1142,7 +1181,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="8"/>
       <c r="E7" s="3" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1153,7 +1192,7 @@
       <c r="C8" s="4"/>
       <c r="D8" s="8"/>
       <c r="E8" s="3" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1286,16 +1325,16 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="39.0"/>
-    <col min="2" max="2" customWidth="true" width="29.5703125"/>
-    <col min="3" max="3" customWidth="true" width="36.28515625"/>
-    <col min="4" max="4" customWidth="true" width="26.28515625"/>
-    <col min="5" max="5" style="5" width="9.140625"/>
+    <col min="1" max="1" width="39" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1320,7 +1359,7 @@
         <v>84</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>63</v>
@@ -1346,15 +1385,15 @@
         <v>63</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="23" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>63</v>
@@ -1400,7 +1439,7 @@
         <v>63</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>63</v>
@@ -1417,7 +1456,7 @@
         <v>63</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>63</v>
@@ -1496,16 +1535,16 @@
     </row>
     <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>63</v>
@@ -1513,16 +1552,16 @@
     </row>
     <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="21" t="s">
-        <v>92</v>
-      </c>
       <c r="C14" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E14" s="9"/>
     </row>
@@ -1541,15 +1580,15 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="20.7109375"/>
-    <col min="2" max="2" customWidth="true" width="20.0"/>
-    <col min="3" max="3" customWidth="true" width="22.42578125"/>
-    <col min="4" max="4" customWidth="true" width="29.7109375"/>
+    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
@@ -1727,4 +1766,151 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6730126F-3340-4E64-9F05-F2B18BD3B5B1}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="27"/>
+    </row>
+    <row r="17" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update connect db , search test SA_11,12,13,14
</commit_message>
<xml_diff>
--- a/data/DataTestOnplus.xlsx
+++ b/data/DataTestOnplus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\automation-appium\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E057D3-AAD7-4FBC-B6B9-FD861CCED63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88111B32-46E2-41D6-A1D7-F06F6B70A20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9030" yWindow="2505" windowWidth="21000" windowHeight="12165" activeTab="4" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
+    <workbookView xWindow="5025" yWindow="2895" windowWidth="21000" windowHeight="12165" activeTab="4" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -1773,7 +1773,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update search test SA_18,27,28.
</commit_message>
<xml_diff>
--- a/data/DataTestOnplus.xlsx
+++ b/data/DataTestOnplus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\automation-appium\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7290B46B-9E9C-41A6-826E-D820E0CC64C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD5B48D-8A47-4090-9F65-C74060D6BF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12540" yWindow="2115" windowWidth="15330" windowHeight="10890" activeTab="4" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="114">
   <si>
     <t>Test case</t>
   </si>
@@ -365,6 +365,12 @@
   </si>
   <si>
     <t xml:space="preserve">#@1234 </t>
+  </si>
+  <si>
+    <t>SA_17</t>
+  </si>
+  <si>
+    <t>SA_18</t>
   </si>
 </sst>
 </file>
@@ -530,7 +536,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1732,10 +1738,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6730126F-3340-4E64-9F05-F2B18BD3B5B1}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,7 +1759,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1761,7 +1767,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1769,7 +1775,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="3" t="s">
         <v>103</v>
       </c>
       <c r="B4" s="27" t="s">
@@ -1777,23 +1783,23 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="14">
         <v>1234567</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="14" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B7" s="28" t="s">
@@ -1801,8 +1807,26 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
update search test SA_1,2,19
</commit_message>
<xml_diff>
--- a/data/DataTestOnplus.xlsx
+++ b/data/DataTestOnplus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\automation-appium\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD5B48D-8A47-4090-9F65-C74060D6BF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07AAF97-3275-42B7-B65E-16CC697346D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12540" yWindow="2115" windowWidth="15330" windowHeight="10890" activeTab="4" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4F8C7B64-1DF0-4A3B-ADCB-899EC34426F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="115">
   <si>
     <t>Test case</t>
   </si>
@@ -371,6 +371,9 @@
   </si>
   <si>
     <t>SA_18</t>
+  </si>
+  <si>
+    <t>Giải đấu</t>
   </si>
 </sst>
 </file>
@@ -1741,7 +1744,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1817,7 +1820,7 @@
         <v>113</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">

</xml_diff>